<commit_message>
implemented reading scenario data from csv
</commit_message>
<xml_diff>
--- a/Event_system/Event_system/docs/ScenarioData.xlsx
+++ b/Event_system/Event_system/docs/ScenarioData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="13240" yWindow="680" windowWidth="12840" windowHeight="9080" tabRatio="500"/>
+    <workbookView xWindow="5720" yWindow="0" windowWidth="20860" windowHeight="11740" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="ScenarioTexts" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
   <si>
     <t>ScenarioName</t>
   </si>
@@ -37,9 +37,6 @@
     <t>Marry partner</t>
   </si>
   <si>
-    <t>Yes, No</t>
-  </si>
-  <si>
     <t>ScenarioId</t>
   </si>
   <si>
@@ -53,6 +50,57 @@
   </si>
   <si>
     <t>ScenarioScope</t>
+  </si>
+  <si>
+    <t>ScenarioItemCount</t>
+  </si>
+  <si>
+    <t>ScenarioItem1</t>
+  </si>
+  <si>
+    <t>ScenarioItem2</t>
+  </si>
+  <si>
+    <t>ScenarioItem3</t>
+  </si>
+  <si>
+    <t>ScenarioItem4</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes, but…</t>
+  </si>
+  <si>
+    <t>No, but…</t>
+  </si>
+  <si>
+    <t>Ragnar</t>
+  </si>
+  <si>
+    <t>Lagertha</t>
+  </si>
+  <si>
+    <t>Widow</t>
+  </si>
+  <si>
+    <t>Deceased</t>
+  </si>
+  <si>
+    <t>Champion1</t>
+  </si>
+  <si>
+    <t>Champion2</t>
+  </si>
+  <si>
+    <t>Champion3</t>
+  </si>
+  <si>
+    <t>Champion4</t>
   </si>
 </sst>
 </file>
@@ -101,8 +149,30 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -121,7 +191,7 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="37">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -129,6 +199,17 @@
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -136,6 +217,17 @@
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -465,22 +557,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="10" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -489,10 +583,40 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N1" t="s">
+        <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:14">
       <c r="A2">
         <v>1</v>
       </c>
@@ -502,22 +626,67 @@
       <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" t="s">
-        <v>5</v>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" t="s">
+        <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:14">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>5</v>
+      <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>4</v>
+      </c>
+      <c r="G3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3" t="s">
+        <v>19</v>
+      </c>
+      <c r="L3" t="s">
+        <v>21</v>
+      </c>
+      <c r="M3" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -535,7 +704,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -546,13 +717,13 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
         <v>9</v>
-      </c>
-      <c r="C1" t="s">
-        <v>10</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>

</xml_diff>